<commit_message>
added test data for negative testing
</commit_message>
<xml_diff>
--- a/testData/LoginData.xlsx
+++ b/testData/LoginData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>emailAddress</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>nagid86419@cybtric.com</t>
+  </si>
+  <si>
+    <t>krthik234@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1188,13 +1191,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1212,6 +1215,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>